<commit_message>
Avancement interface compilation pointage + Ajax changement date compilation + Avancement Ajax sauvegarde modification sur compilation.
</commit_message>
<xml_diff>
--- a/Symfony/Validation Manager WF RF MAJ NR 300516.xlsx
+++ b/Symfony/Validation Manager WF RF MAJ NR 300516.xlsx
@@ -2506,6 +2506,9 @@
     <t>00000089</t>
   </si>
   <si>
+    <t>Tristan BESSON</t>
+  </si>
+  <si>
     <t>00000466</t>
   </si>
   <si>
@@ -3320,9 +3323,6 @@
   </si>
   <si>
     <t>REGIS</t>
-  </si>
-  <si>
-    <t>Tristan BESSON</t>
   </si>
 </sst>
 </file>
@@ -3333,7 +3333,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -3395,6 +3395,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -3518,7 +3523,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3583,6 +3588,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3603,7 +3612,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Good" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -3675,27 +3684,27 @@
   </sheetPr>
   <dimension ref="A1:N399"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A381" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G399" activeCellId="0" sqref="G399"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A283" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G290" activeCellId="0" sqref="G290"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.1326530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="256" min="10" style="1" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="1" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.7295918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="256" min="10" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="1" width="10.9336734693878"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="2" s="2" customFormat="true" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -3707,8 +3716,9 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
-    </row>
-    <row r="3" s="2" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N2" s="0"/>
+    </row>
+    <row r="3" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -3720,8 +3730,9 @@
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="I3" s="6"/>
-    </row>
-    <row r="4" s="2" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N3" s="0"/>
+    </row>
+    <row r="4" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -3749,6 +3760,7 @@
       <c r="I4" s="9" t="s">
         <v>10</v>
       </c>
+      <c r="N4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
@@ -12364,8 +12376,8 @@
       <c r="F294" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G294" s="13" t="s">
-        <v>84</v>
+      <c r="G294" s="16" t="s">
+        <v>827</v>
       </c>
       <c r="H294" s="11" t="s">
         <v>820</v>
@@ -12382,13 +12394,13 @@
         <v>786</v>
       </c>
       <c r="C295" s="11" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="D295" s="11" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="E295" s="11" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="F295" s="11" t="s">
         <v>34</v>
@@ -12411,10 +12423,10 @@
         <v>786</v>
       </c>
       <c r="C296" s="11" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="D296" s="11" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="E296" s="11" t="s">
         <v>748</v>
@@ -12426,7 +12438,7 @@
         <v>84</v>
       </c>
       <c r="H296" s="11" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="I296" s="12" t="s">
         <v>86</v>
@@ -12440,13 +12452,13 @@
         <v>786</v>
       </c>
       <c r="C297" s="11" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="D297" s="11" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="E297" s="11" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="F297" s="11" t="s">
         <v>16</v>
@@ -12469,13 +12481,13 @@
         <v>786</v>
       </c>
       <c r="C298" s="11" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="D298" s="11" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="E298" s="11" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="F298" s="11" t="s">
         <v>16</v>
@@ -12498,13 +12510,13 @@
         <v>786</v>
       </c>
       <c r="C299" s="11" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="D299" s="11" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="E299" s="11" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="F299" s="11" t="s">
         <v>16</v>
@@ -12527,13 +12539,13 @@
         <v>786</v>
       </c>
       <c r="C300" s="11" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="D300" s="11" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="E300" s="11" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="F300" s="11" t="s">
         <v>16</v>
@@ -12556,13 +12568,13 @@
         <v>786</v>
       </c>
       <c r="C301" s="11" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="D301" s="11" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="E301" s="11" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="F301" s="11" t="s">
         <v>16</v>
@@ -12585,13 +12597,13 @@
         <v>786</v>
       </c>
       <c r="C302" s="11" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="D302" s="11" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="E302" s="11" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="F302" s="11" t="s">
         <v>16</v>
@@ -12614,10 +12626,10 @@
         <v>786</v>
       </c>
       <c r="C303" s="11" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="D303" s="11" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="E303" s="11" t="s">
         <v>78</v>
@@ -12640,22 +12652,22 @@
         <v>252</v>
       </c>
       <c r="B304" s="11" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="C304" s="11" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="D304" s="11" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="E304" s="11" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="F304" s="11" t="s">
         <v>16</v>
       </c>
       <c r="G304" s="11" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="H304" s="11" t="s">
         <v>18</v>
@@ -12669,25 +12681,25 @@
         <v>252</v>
       </c>
       <c r="B305" s="11" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="C305" s="11" t="s">
+        <v>859</v>
+      </c>
+      <c r="D305" s="11" t="s">
+        <v>860</v>
+      </c>
+      <c r="E305" s="11" t="s">
+        <v>861</v>
+      </c>
+      <c r="F305" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G305" s="11" t="s">
         <v>858</v>
       </c>
-      <c r="D305" s="11" t="s">
-        <v>859</v>
-      </c>
-      <c r="E305" s="11" t="s">
-        <v>860</v>
-      </c>
-      <c r="F305" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G305" s="11" t="s">
-        <v>857</v>
-      </c>
       <c r="H305" s="11" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="I305" s="12" t="s">
         <v>106</v>
@@ -12698,25 +12710,25 @@
         <v>252</v>
       </c>
       <c r="B306" s="11" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="C306" s="11" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="D306" s="11" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="E306" s="11" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="F306" s="11" t="s">
         <v>62</v>
       </c>
       <c r="G306" s="11" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="H306" s="11" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="I306" s="12" t="s">
         <v>106</v>
@@ -12727,25 +12739,25 @@
         <v>252</v>
       </c>
       <c r="B307" s="11" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="C307" s="11" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="D307" s="11" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="E307" s="11" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="F307" s="11" t="s">
         <v>16</v>
       </c>
       <c r="G307" s="11" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="H307" s="11" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="I307" s="12" t="s">
         <v>106</v>
@@ -12756,13 +12768,13 @@
         <v>252</v>
       </c>
       <c r="B308" s="11" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="C308" s="11" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="D308" s="11" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="E308" s="11" t="s">
         <v>299</v>
@@ -12771,10 +12783,10 @@
         <v>16</v>
       </c>
       <c r="G308" s="11" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="H308" s="11" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="I308" s="12" t="s">
         <v>106</v>
@@ -12785,25 +12797,25 @@
         <v>252</v>
       </c>
       <c r="B309" s="11" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="C309" s="11" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="D309" s="11" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="E309" s="11" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="F309" s="11" t="s">
         <v>16</v>
       </c>
       <c r="G309" s="11" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="H309" s="11" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="I309" s="12" t="s">
         <v>106</v>
@@ -12814,13 +12826,13 @@
         <v>252</v>
       </c>
       <c r="B310" s="11" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="C310" s="11" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="D310" s="11" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="E310" s="11" t="s">
         <v>420</v>
@@ -12829,10 +12841,10 @@
         <v>16</v>
       </c>
       <c r="G310" s="11" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="H310" s="11" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="I310" s="12" t="s">
         <v>106</v>
@@ -12843,25 +12855,25 @@
         <v>252</v>
       </c>
       <c r="B311" s="11" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="C311" s="11" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="D311" s="11" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="E311" s="11" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="F311" s="11" t="s">
         <v>16</v>
       </c>
       <c r="G311" s="11" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="H311" s="11" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="I311" s="12" t="s">
         <v>106</v>
@@ -12872,25 +12884,25 @@
         <v>252</v>
       </c>
       <c r="B312" s="11" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="C312" s="11" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="D312" s="11" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="E312" s="11" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="F312" s="11" t="s">
         <v>62</v>
       </c>
       <c r="G312" s="11" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="H312" s="11" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="I312" s="12" t="s">
         <v>106</v>
@@ -12901,13 +12913,13 @@
         <v>252</v>
       </c>
       <c r="B313" s="11" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="C313" s="11" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="D313" s="11" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="E313" s="11" t="s">
         <v>398</v>
@@ -12916,10 +12928,10 @@
         <v>16</v>
       </c>
       <c r="G313" s="11" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="H313" s="11" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="I313" s="12" t="s">
         <v>106</v>
@@ -12930,13 +12942,13 @@
         <v>252</v>
       </c>
       <c r="B314" s="11" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="C314" s="11" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="D314" s="11" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="E314" s="11" t="s">
         <v>447</v>
@@ -12945,10 +12957,10 @@
         <v>16</v>
       </c>
       <c r="G314" s="11" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="H314" s="11" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="I314" s="12" t="s">
         <v>106</v>
@@ -12956,19 +12968,19 @@
     </row>
     <row r="315" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A315" s="10" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="B315" s="11" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="C315" s="11" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="D315" s="11" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="E315" s="11" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="F315" s="11" t="s">
         <v>16</v>
@@ -12985,19 +12997,19 @@
     </row>
     <row r="316" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A316" s="10" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="B316" s="11" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="C316" s="11" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="D316" s="11" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="E316" s="11" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="F316" s="11" t="s">
         <v>16</v>
@@ -13014,16 +13026,16 @@
     </row>
     <row r="317" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A317" s="10" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="B317" s="11" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="C317" s="11" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="D317" s="11" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="E317" s="11" t="s">
         <v>555</v>
@@ -13043,16 +13055,16 @@
     </row>
     <row r="318" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A318" s="10" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="B318" s="11" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="C318" s="11" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="D318" s="11" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="E318" s="11" t="s">
         <v>305</v>
@@ -13072,19 +13084,19 @@
     </row>
     <row r="319" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A319" s="10" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="B319" s="11" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="C319" s="11" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="D319" s="11" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="E319" s="11" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="F319" s="11" t="s">
         <v>16</v>
@@ -13101,16 +13113,16 @@
     </row>
     <row r="320" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A320" s="10" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="B320" s="11" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="C320" s="11" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="D320" s="11" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="E320" s="11" t="s">
         <v>363</v>
@@ -13122,7 +13134,7 @@
         <v>84</v>
       </c>
       <c r="H320" s="11" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="I320" s="12" t="s">
         <v>86</v>
@@ -13130,19 +13142,19 @@
     </row>
     <row r="321" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A321" s="10" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="B321" s="11" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="C321" s="11" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="D321" s="11" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="E321" s="11" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="F321" s="11" t="s">
         <v>16</v>
@@ -13159,16 +13171,16 @@
     </row>
     <row r="322" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A322" s="10" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="B322" s="11" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="C322" s="11" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="D322" s="11" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="E322" s="11" t="s">
         <v>527</v>
@@ -13180,7 +13192,7 @@
         <v>84</v>
       </c>
       <c r="H322" s="11" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="I322" s="12" t="s">
         <v>86</v>
@@ -13188,16 +13200,16 @@
     </row>
     <row r="323" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A323" s="10" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="B323" s="11" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="C323" s="11" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="D323" s="11" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="E323" s="11" t="s">
         <v>595</v>
@@ -13209,7 +13221,7 @@
         <v>84</v>
       </c>
       <c r="H323" s="11" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="I323" s="12" t="s">
         <v>86</v>
@@ -13217,16 +13229,16 @@
     </row>
     <row r="324" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A324" s="10" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="B324" s="11" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="C324" s="11" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="D324" s="11" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="E324" s="11" t="s">
         <v>784</v>
@@ -13238,7 +13250,7 @@
         <v>84</v>
       </c>
       <c r="H324" s="11" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="I324" s="12" t="s">
         <v>86</v>
@@ -13246,16 +13258,16 @@
     </row>
     <row r="325" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A325" s="10" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="B325" s="11" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="C325" s="11" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="D325" s="11" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="E325" s="11" t="s">
         <v>162</v>
@@ -13267,7 +13279,7 @@
         <v>84</v>
       </c>
       <c r="H325" s="11" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="I325" s="12" t="s">
         <v>86</v>
@@ -13275,19 +13287,19 @@
     </row>
     <row r="326" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A326" s="10" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="B326" s="11" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="C326" s="11" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="D326" s="11" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="E326" s="11" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="F326" s="11" t="s">
         <v>34</v>
@@ -13304,19 +13316,19 @@
     </row>
     <row r="327" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A327" s="10" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="B327" s="11" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="C327" s="11" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="D327" s="11" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="E327" s="11" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="F327" s="11" t="s">
         <v>16</v>
@@ -13325,7 +13337,7 @@
         <v>84</v>
       </c>
       <c r="H327" s="11" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="I327" s="12" t="s">
         <v>86</v>
@@ -13333,16 +13345,16 @@
     </row>
     <row r="328" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A328" s="10" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="B328" s="11" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="C328" s="11" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="D328" s="11" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="E328" s="11" t="s">
         <v>78</v>
@@ -13350,11 +13362,11 @@
       <c r="F328" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G328" s="13" t="s">
-        <v>84</v>
+      <c r="G328" s="16" t="s">
+        <v>827</v>
       </c>
       <c r="H328" s="11" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="I328" s="12" t="s">
         <v>86</v>
@@ -13362,16 +13374,16 @@
     </row>
     <row r="329" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A329" s="10" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="B329" s="11" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="C329" s="11" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="D329" s="11" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="E329" s="11" t="s">
         <v>299</v>
@@ -13383,7 +13395,7 @@
         <v>84</v>
       </c>
       <c r="H329" s="11" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="I329" s="12" t="s">
         <v>86</v>
@@ -13391,16 +13403,16 @@
     </row>
     <row r="330" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A330" s="10" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="B330" s="11" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="C330" s="11" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="D330" s="11" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="E330" s="11" t="s">
         <v>635</v>
@@ -13412,7 +13424,7 @@
         <v>84</v>
       </c>
       <c r="H330" s="11" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="I330" s="12" t="s">
         <v>86</v>
@@ -13420,19 +13432,19 @@
     </row>
     <row r="331" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A331" s="10" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="B331" s="11" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="C331" s="11" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="D331" s="11" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="E331" s="11" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="F331" s="11" t="s">
         <v>16</v>
@@ -13441,7 +13453,7 @@
         <v>84</v>
       </c>
       <c r="H331" s="11" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="I331" s="12" t="s">
         <v>86</v>
@@ -13449,16 +13461,16 @@
     </row>
     <row r="332" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A332" s="10" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="B332" s="11" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="C332" s="11" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="D332" s="11" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="E332" s="11" t="s">
         <v>825</v>
@@ -13470,7 +13482,7 @@
         <v>84</v>
       </c>
       <c r="H332" s="11" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="I332" s="12" t="s">
         <v>86</v>
@@ -13478,19 +13490,19 @@
     </row>
     <row r="333" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A333" s="10" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="B333" s="11" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="C333" s="11" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="D333" s="11" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="E333" s="11" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="F333" s="11" t="s">
         <v>16</v>
@@ -13499,7 +13511,7 @@
         <v>84</v>
       </c>
       <c r="H333" s="11" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="I333" s="12" t="s">
         <v>86</v>
@@ -13507,19 +13519,19 @@
     </row>
     <row r="334" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A334" s="10" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="B334" s="11" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="C334" s="11" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="D334" s="11" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="E334" s="11" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="F334" s="11" t="s">
         <v>16</v>
@@ -13528,7 +13540,7 @@
         <v>84</v>
       </c>
       <c r="H334" s="11" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="I334" s="12" t="s">
         <v>86</v>
@@ -13536,19 +13548,19 @@
     </row>
     <row r="335" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A335" s="10" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="B335" s="11" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="C335" s="11" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="D335" s="11" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="E335" s="11" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="F335" s="11" t="s">
         <v>16</v>
@@ -13557,7 +13569,7 @@
         <v>84</v>
       </c>
       <c r="H335" s="11" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="I335" s="12" t="s">
         <v>86</v>
@@ -13565,19 +13577,19 @@
     </row>
     <row r="336" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A336" s="10" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="B336" s="11" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="C336" s="11" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="D336" s="11" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="E336" s="11" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="F336" s="11" t="s">
         <v>16</v>
@@ -13586,7 +13598,7 @@
         <v>84</v>
       </c>
       <c r="H336" s="11" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="I336" s="12" t="s">
         <v>86</v>
@@ -13594,19 +13606,19 @@
     </row>
     <row r="337" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A337" s="10" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="B337" s="11" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="C337" s="11" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="D337" s="11" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="E337" s="11" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="F337" s="11" t="s">
         <v>16</v>
@@ -13615,7 +13627,7 @@
         <v>84</v>
       </c>
       <c r="H337" s="11" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="I337" s="12" t="s">
         <v>86</v>
@@ -13623,19 +13635,19 @@
     </row>
     <row r="338" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A338" s="10" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="B338" s="11" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="C338" s="11" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="D338" s="11" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="E338" s="11" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="F338" s="11" t="s">
         <v>16</v>
@@ -13644,7 +13656,7 @@
         <v>84</v>
       </c>
       <c r="H338" s="11" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="I338" s="12" t="s">
         <v>86</v>
@@ -13652,16 +13664,16 @@
     </row>
     <row r="339" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A339" s="10" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="B339" s="11" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="C339" s="11" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="D339" s="11" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="E339" s="11" t="s">
         <v>61</v>
@@ -13673,7 +13685,7 @@
         <v>84</v>
       </c>
       <c r="H339" s="11" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="I339" s="12" t="s">
         <v>86</v>
@@ -13681,19 +13693,19 @@
     </row>
     <row r="340" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A340" s="10" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="B340" s="11" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="C340" s="11" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="D340" s="11" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="E340" s="11" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="F340" s="11" t="s">
         <v>34</v>
@@ -13702,7 +13714,7 @@
         <v>84</v>
       </c>
       <c r="H340" s="11" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="I340" s="12" t="s">
         <v>86</v>
@@ -13710,19 +13722,19 @@
     </row>
     <row r="341" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A341" s="10" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="B341" s="11" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="C341" s="11" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="D341" s="11" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="E341" s="11" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="F341" s="11" t="s">
         <v>16</v>
@@ -13731,7 +13743,7 @@
         <v>84</v>
       </c>
       <c r="H341" s="11" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="I341" s="12" t="s">
         <v>86</v>
@@ -13739,19 +13751,19 @@
     </row>
     <row r="342" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A342" s="10" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="B342" s="11" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="C342" s="11" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="D342" s="11" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="E342" s="11" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="F342" s="11" t="s">
         <v>16</v>
@@ -13760,7 +13772,7 @@
         <v>84</v>
       </c>
       <c r="H342" s="11" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="I342" s="12" t="s">
         <v>86</v>
@@ -13771,13 +13783,13 @@
         <v>11</v>
       </c>
       <c r="B343" s="11" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="C343" s="11" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="D343" s="11" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="E343" s="11" t="s">
         <v>22</v>
@@ -13800,22 +13812,22 @@
         <v>11</v>
       </c>
       <c r="B344" s="11" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="C344" s="11" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="D344" s="11" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="E344" s="11" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="F344" s="11" t="s">
         <v>16</v>
       </c>
       <c r="G344" s="11" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="H344" s="11" t="s">
         <v>27</v>
@@ -13829,13 +13841,13 @@
         <v>11</v>
       </c>
       <c r="B345" s="11" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="C345" s="11" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="D345" s="11" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="E345" s="11" t="s">
         <v>370</v>
@@ -13844,7 +13856,7 @@
         <v>16</v>
       </c>
       <c r="G345" s="11" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="H345" s="11" t="s">
         <v>27</v>
@@ -13858,13 +13870,13 @@
         <v>11</v>
       </c>
       <c r="B346" s="11" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="C346" s="11" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="D346" s="11" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="E346" s="11" t="s">
         <v>22</v>
@@ -13873,7 +13885,7 @@
         <v>34</v>
       </c>
       <c r="G346" s="11" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="H346" s="11" t="s">
         <v>27</v>
@@ -13887,22 +13899,22 @@
         <v>11</v>
       </c>
       <c r="B347" s="11" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="C347" s="11" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="D347" s="11" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="E347" s="11" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="F347" s="11" t="s">
         <v>16</v>
       </c>
       <c r="G347" s="11" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="H347" s="11" t="s">
         <v>27</v>
@@ -13916,22 +13928,22 @@
         <v>11</v>
       </c>
       <c r="B348" s="11" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="C348" s="11" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="D348" s="11" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="E348" s="11" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="F348" s="11" t="s">
         <v>46</v>
       </c>
       <c r="G348" s="11" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="H348" s="11" t="s">
         <v>27</v>
@@ -13945,10 +13957,10 @@
         <v>11</v>
       </c>
       <c r="B349" s="11" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="C349" s="11" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="D349" s="11" t="s">
         <v>613</v>
@@ -13960,7 +13972,7 @@
         <v>16</v>
       </c>
       <c r="G349" s="11" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="H349" s="11" t="s">
         <v>27</v>
@@ -13974,13 +13986,13 @@
         <v>11</v>
       </c>
       <c r="B350" s="11" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="C350" s="11" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="D350" s="11" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="E350" s="11" t="s">
         <v>370</v>
@@ -13989,7 +14001,7 @@
         <v>16</v>
       </c>
       <c r="G350" s="11" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="H350" s="11" t="s">
         <v>27</v>
@@ -14003,13 +14015,13 @@
         <v>11</v>
       </c>
       <c r="B351" s="11" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="C351" s="11" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="D351" s="11" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="E351" s="11" t="s">
         <v>627</v>
@@ -14018,7 +14030,7 @@
         <v>16</v>
       </c>
       <c r="G351" s="11" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="H351" s="11" t="s">
         <v>27</v>
@@ -14029,25 +14041,25 @@
     </row>
     <row r="352" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A352" s="10" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="B352" s="11" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="C352" s="11" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="D352" s="11" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="E352" s="11" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="F352" s="11" t="s">
         <v>16</v>
       </c>
       <c r="G352" s="11" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="H352" s="11" t="s">
         <v>667</v>
@@ -14058,16 +14070,16 @@
     </row>
     <row r="353" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A353" s="10" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="B353" s="11" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="C353" s="11" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="D353" s="11" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="E353" s="11" t="s">
         <v>52</v>
@@ -14076,7 +14088,7 @@
         <v>16</v>
       </c>
       <c r="G353" s="11" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="H353" s="11" t="s">
         <v>667</v>
@@ -14087,16 +14099,16 @@
     </row>
     <row r="354" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A354" s="10" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="B354" s="11" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="C354" s="11" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="D354" s="11" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="E354" s="11" t="s">
         <v>214</v>
@@ -14105,7 +14117,7 @@
         <v>16</v>
       </c>
       <c r="G354" s="11" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="H354" s="11" t="s">
         <v>667</v>
@@ -14116,28 +14128,28 @@
     </row>
     <row r="355" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A355" s="10" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="B355" s="11" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="C355" s="11" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="D355" s="11" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="E355" s="11" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="F355" s="11" t="s">
         <v>16</v>
       </c>
       <c r="G355" s="11" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="H355" s="11" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="I355" s="12" t="s">
         <v>19</v>
@@ -14145,28 +14157,28 @@
     </row>
     <row r="356" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A356" s="10" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="B356" s="11" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="C356" s="11" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="D356" s="11" t="s">
         <v>675</v>
       </c>
       <c r="E356" s="11" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="F356" s="11" t="s">
         <v>16</v>
       </c>
       <c r="G356" s="11" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="H356" s="11" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="I356" s="12" t="s">
         <v>19</v>
@@ -14174,28 +14186,28 @@
     </row>
     <row r="357" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A357" s="10" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="B357" s="11" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="C357" s="11" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="D357" s="11" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="E357" s="11" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="F357" s="11" t="s">
         <v>16</v>
       </c>
       <c r="G357" s="11" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="H357" s="11" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="I357" s="12" t="s">
         <v>19</v>
@@ -14203,28 +14215,28 @@
     </row>
     <row r="358" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A358" s="10" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="B358" s="11" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="C358" s="11" t="s">
+        <v>1007</v>
+      </c>
+      <c r="D358" s="11" t="s">
+        <v>1008</v>
+      </c>
+      <c r="E358" s="11" t="s">
+        <v>1009</v>
+      </c>
+      <c r="F358" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G358" s="11" t="s">
+        <v>993</v>
+      </c>
+      <c r="H358" s="11" t="s">
         <v>1006</v>
-      </c>
-      <c r="D358" s="11" t="s">
-        <v>1007</v>
-      </c>
-      <c r="E358" s="11" t="s">
-        <v>1008</v>
-      </c>
-      <c r="F358" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G358" s="11" t="s">
-        <v>992</v>
-      </c>
-      <c r="H358" s="11" t="s">
-        <v>1005</v>
       </c>
       <c r="I358" s="12" t="s">
         <v>19</v>
@@ -14232,16 +14244,16 @@
     </row>
     <row r="359" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A359" s="10" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="B359" s="11" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="C359" s="11" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="D359" s="11" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="E359" s="11" t="s">
         <v>595</v>
@@ -14250,10 +14262,10 @@
         <v>16</v>
       </c>
       <c r="G359" s="11" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="H359" s="11" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="I359" s="12" t="s">
         <v>19</v>
@@ -14261,16 +14273,16 @@
     </row>
     <row r="360" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A360" s="10" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="B360" s="11" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="C360" s="11" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="D360" s="11" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="E360" s="11" t="s">
         <v>287</v>
@@ -14279,10 +14291,10 @@
         <v>16</v>
       </c>
       <c r="G360" s="11" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="H360" s="11" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="I360" s="12" t="s">
         <v>19</v>
@@ -14290,16 +14302,16 @@
     </row>
     <row r="361" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A361" s="10" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="B361" s="11" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="C361" s="11" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="D361" s="11" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="E361" s="11" t="s">
         <v>115</v>
@@ -14308,10 +14320,10 @@
         <v>16</v>
       </c>
       <c r="G361" s="11" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="H361" s="11" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="I361" s="12" t="s">
         <v>19</v>
@@ -14319,16 +14331,16 @@
     </row>
     <row r="362" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A362" s="10" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="B362" s="11" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="C362" s="11" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="D362" s="11" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="E362" s="11" t="s">
         <v>227</v>
@@ -14337,10 +14349,10 @@
         <v>16</v>
       </c>
       <c r="G362" s="11" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="H362" s="11" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="I362" s="12" t="s">
         <v>19</v>
@@ -14348,16 +14360,16 @@
     </row>
     <row r="363" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A363" s="10" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="B363" s="11" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="C363" s="11" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="D363" s="11" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="E363" s="11" t="s">
         <v>646</v>
@@ -14366,10 +14378,10 @@
         <v>16</v>
       </c>
       <c r="G363" s="11" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="H363" s="11" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="I363" s="12" t="s">
         <v>19</v>
@@ -14377,28 +14389,28 @@
     </row>
     <row r="364" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A364" s="10" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="B364" s="11" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="C364" s="11" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="D364" s="11" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="E364" s="11" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="F364" s="11" t="s">
         <v>16</v>
       </c>
       <c r="G364" s="11" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="H364" s="11" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="I364" s="12" t="s">
         <v>19</v>
@@ -14406,28 +14418,28 @@
     </row>
     <row r="365" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A365" s="10" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="B365" s="11" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="C365" s="11" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="D365" s="11" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="E365" s="11" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="F365" s="11" t="s">
         <v>16</v>
       </c>
       <c r="G365" s="11" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="H365" s="11" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="I365" s="12" t="s">
         <v>19</v>
@@ -14435,16 +14447,16 @@
     </row>
     <row r="366" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A366" s="10" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="B366" s="11" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="C366" s="11" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="D366" s="11" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="E366" s="11" t="s">
         <v>395</v>
@@ -14453,10 +14465,10 @@
         <v>16</v>
       </c>
       <c r="G366" s="11" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="H366" s="11" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="I366" s="12" t="s">
         <v>19</v>
@@ -14464,10 +14476,10 @@
     </row>
     <row r="367" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A367" s="10" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="B367" s="11" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="C367" s="14"/>
       <c r="D367" s="14" t="s">
@@ -14480,10 +14492,10 @@
         <v>16</v>
       </c>
       <c r="G367" s="11" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="H367" s="11" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="I367" s="12" t="s">
         <v>19</v>
@@ -14491,26 +14503,26 @@
     </row>
     <row r="368" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A368" s="10" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="B368" s="11" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="C368" s="14"/>
       <c r="D368" s="14" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="E368" s="14" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="F368" s="14" t="s">
         <v>34</v>
       </c>
       <c r="G368" s="11" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="H368" s="11" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="I368" s="12" t="s">
         <v>19</v>
@@ -14521,25 +14533,25 @@
         <v>63</v>
       </c>
       <c r="B369" s="11" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="C369" s="11" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="D369" s="11" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="E369" s="11" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="F369" s="11" t="s">
         <v>16</v>
       </c>
       <c r="G369" s="11" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="H369" s="11" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="I369" s="12" t="s">
         <v>19</v>
@@ -14550,13 +14562,13 @@
         <v>63</v>
       </c>
       <c r="B370" s="11" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="C370" s="11" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="D370" s="11" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="E370" s="11" t="s">
         <v>389</v>
@@ -14565,10 +14577,10 @@
         <v>62</v>
       </c>
       <c r="G370" s="11" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="H370" s="11" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="I370" s="12" t="s">
         <v>19</v>
@@ -14579,25 +14591,25 @@
         <v>63</v>
       </c>
       <c r="B371" s="11" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="C371" s="11" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="D371" s="11" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="E371" s="11" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c r="F371" s="11" t="s">
         <v>16</v>
       </c>
       <c r="G371" s="11" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="H371" s="11" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="I371" s="12" t="s">
         <v>19</v>
@@ -14608,13 +14620,13 @@
         <v>63</v>
       </c>
       <c r="B372" s="11" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="C372" s="11" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="D372" s="11" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="E372" s="11" t="s">
         <v>256</v>
@@ -14623,10 +14635,10 @@
         <v>16</v>
       </c>
       <c r="G372" s="11" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="H372" s="11" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="I372" s="12" t="s">
         <v>19</v>
@@ -14637,25 +14649,25 @@
         <v>63</v>
       </c>
       <c r="B373" s="11" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="C373" s="11" t="s">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="D373" s="11" t="s">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="E373" s="11" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="F373" s="11" t="s">
         <v>16</v>
       </c>
       <c r="G373" s="11" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="H373" s="11" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="I373" s="12" t="s">
         <v>19</v>
@@ -14666,13 +14678,13 @@
         <v>63</v>
       </c>
       <c r="B374" s="11" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="C374" s="11" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="D374" s="11" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="E374" s="11" t="s">
         <v>555</v>
@@ -14681,10 +14693,10 @@
         <v>16</v>
       </c>
       <c r="G374" s="11" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="H374" s="11" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="I374" s="12" t="s">
         <v>19</v>
@@ -14695,13 +14707,13 @@
         <v>63</v>
       </c>
       <c r="B375" s="11" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="C375" s="11" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="D375" s="11" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="E375" s="11" t="s">
         <v>167</v>
@@ -14710,10 +14722,10 @@
         <v>16</v>
       </c>
       <c r="G375" s="11" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="H375" s="11" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="I375" s="12" t="s">
         <v>19</v>
@@ -14724,13 +14736,13 @@
         <v>63</v>
       </c>
       <c r="B376" s="11" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="C376" s="11" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="D376" s="11" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="E376" s="11" t="s">
         <v>666</v>
@@ -14739,7 +14751,7 @@
         <v>16</v>
       </c>
       <c r="G376" s="11" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="H376" s="11" t="s">
         <v>79</v>
@@ -14753,13 +14765,13 @@
         <v>63</v>
       </c>
       <c r="B377" s="11" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="C377" s="11" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="D377" s="11" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="E377" s="11" t="s">
         <v>606</v>
@@ -14782,16 +14794,16 @@
         <v>63</v>
       </c>
       <c r="B378" s="11" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="C378" s="11" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="D378" s="11" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="E378" s="11" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="F378" s="11" t="s">
         <v>16</v>
@@ -14811,10 +14823,10 @@
         <v>63</v>
       </c>
       <c r="B379" s="11" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="C379" s="11" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="D379" s="11" t="s">
         <v>296</v>
@@ -14840,13 +14852,13 @@
         <v>63</v>
       </c>
       <c r="B380" s="11" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="C380" s="11" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="D380" s="11" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="E380" s="11" t="s">
         <v>617</v>
@@ -14869,13 +14881,13 @@
         <v>63</v>
       </c>
       <c r="B381" s="11" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="C381" s="11" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="D381" s="11" t="s">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="E381" s="11" t="s">
         <v>361</v>
@@ -14898,13 +14910,13 @@
         <v>63</v>
       </c>
       <c r="B382" s="11" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="C382" s="11" t="s">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="D382" s="11" t="s">
-        <v>1063</v>
+        <v>1064</v>
       </c>
       <c r="E382" s="11" t="s">
         <v>78</v>
@@ -14923,31 +14935,31 @@
       </c>
     </row>
     <row r="383" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A383" s="16" t="s">
+      <c r="A383" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B383" s="17" t="s">
-        <v>1051</v>
-      </c>
-      <c r="C383" s="17" t="s">
-        <v>1064</v>
-      </c>
-      <c r="D383" s="17" t="s">
+      <c r="B383" s="18" t="s">
+        <v>1052</v>
+      </c>
+      <c r="C383" s="18" t="s">
         <v>1065</v>
       </c>
-      <c r="E383" s="17" t="s">
+      <c r="D383" s="18" t="s">
+        <v>1066</v>
+      </c>
+      <c r="E383" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="F383" s="17" t="s">
+      <c r="F383" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="G383" s="17" t="s">
+      <c r="G383" s="18" t="s">
         <v>68</v>
       </c>
       <c r="H383" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="I383" s="18" t="s">
+      <c r="I383" s="19" t="s">
         <v>19</v>
       </c>
     </row>
@@ -14956,13 +14968,13 @@
         <v>63</v>
       </c>
       <c r="B384" s="11" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="C384" s="11" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="D384" s="11" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="E384" s="11" t="s">
         <v>182</v>
@@ -14985,13 +14997,13 @@
         <v>63</v>
       </c>
       <c r="B385" s="11" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="C385" s="11" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="D385" s="11" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
       <c r="E385" s="11" t="s">
         <v>454</v>
@@ -15014,13 +15026,13 @@
         <v>63</v>
       </c>
       <c r="B386" s="11" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="C386" s="11" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="D386" s="11" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="E386" s="11" t="s">
         <v>95</v>
@@ -15043,16 +15055,16 @@
         <v>63</v>
       </c>
       <c r="B387" s="11" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="C387" s="11" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="D387" s="11" t="s">
         <v>179</v>
       </c>
       <c r="E387" s="11" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="F387" s="11" t="s">
         <v>16</v>
@@ -15072,16 +15084,16 @@
         <v>63</v>
       </c>
       <c r="B388" s="11" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="C388" s="11" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="D388" s="11" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="E388" s="11" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="F388" s="11" t="s">
         <v>16</v>
@@ -15101,16 +15113,16 @@
         <v>63</v>
       </c>
       <c r="B389" s="11" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="C389" s="11" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="D389" s="11" t="s">
         <v>682</v>
       </c>
       <c r="E389" s="11" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="F389" s="11" t="s">
         <v>34</v>
@@ -15130,16 +15142,16 @@
         <v>63</v>
       </c>
       <c r="B390" s="11" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="C390" s="11" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="D390" s="11" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="E390" s="11" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="F390" s="11" t="s">
         <v>16</v>
@@ -15159,16 +15171,16 @@
         <v>63</v>
       </c>
       <c r="B391" s="11" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="C391" s="11" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="D391" s="11" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="E391" s="11" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="F391" s="11" t="s">
         <v>16</v>
@@ -15188,13 +15200,13 @@
         <v>63</v>
       </c>
       <c r="B392" s="11" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="C392" s="11" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="D392" s="11" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c r="E392" s="11" t="s">
         <v>115</v>
@@ -15217,16 +15229,16 @@
         <v>63</v>
       </c>
       <c r="B393" s="11" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="C393" s="11" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="D393" s="11" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="E393" s="11" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="F393" s="11" t="s">
         <v>16</v>
@@ -15246,13 +15258,13 @@
         <v>63</v>
       </c>
       <c r="B394" s="11" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="C394" s="11" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
       <c r="D394" s="11" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c r="E394" s="11" t="s">
         <v>256</v>
@@ -15275,16 +15287,16 @@
         <v>63</v>
       </c>
       <c r="B395" s="11" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="C395" s="11" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c r="D395" s="11" t="s">
-        <v>1091</v>
+        <v>1092</v>
       </c>
       <c r="E395" s="11" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="F395" s="11" t="s">
         <v>16</v>
@@ -15304,16 +15316,16 @@
         <v>63</v>
       </c>
       <c r="B396" s="11" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="C396" s="11" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="D396" s="11" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="E396" s="11" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="F396" s="11" t="s">
         <v>16</v>
@@ -15333,10 +15345,10 @@
         <v>63</v>
       </c>
       <c r="B397" s="11" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="C397" s="11" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="D397" s="11" t="s">
         <v>361</v>
@@ -15362,16 +15374,16 @@
         <v>63</v>
       </c>
       <c r="B398" s="10" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="C398" s="11" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="D398" s="11" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="E398" s="11" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="F398" s="11" t="s">
         <v>16</v>
@@ -15391,10 +15403,10 @@
         <v>63</v>
       </c>
       <c r="B399" s="10" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="C399" s="11" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="D399" s="11" t="s">
         <v>542</v>
@@ -15406,7 +15418,7 @@
         <v>16</v>
       </c>
       <c r="G399" s="11" t="s">
-        <v>1099</v>
+        <v>827</v>
       </c>
       <c r="H399" s="11" t="s">
         <v>79</v>

</xml_diff>

<commit_message>
Ajout compilation validation DA/Manager.
</commit_message>
<xml_diff>
--- a/Symfony/Validation Manager WF RF MAJ NR 300516.xlsx
+++ b/Symfony/Validation Manager WF RF MAJ NR 300516.xlsx
@@ -3589,7 +3589,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -3684,23 +3684,23 @@
   </sheetPr>
   <dimension ref="A1:N399"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A283" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G290" activeCellId="0" sqref="G290"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A285" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H295" activeCellId="0" sqref="H295"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.7295918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="256" min="10" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="1" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.3214285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="256" min="10" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="1" width="10.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -12376,11 +12376,11 @@
       <c r="F294" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G294" s="16" t="s">
+      <c r="G294" s="13" t="s">
         <v>827</v>
       </c>
-      <c r="H294" s="11" t="s">
-        <v>820</v>
+      <c r="H294" s="16" t="s">
+        <v>827</v>
       </c>
       <c r="I294" s="12" t="s">
         <v>86</v>
@@ -13362,11 +13362,11 @@
       <c r="F328" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G328" s="16" t="s">
+      <c r="G328" s="13" t="s">
         <v>827</v>
       </c>
-      <c r="H328" s="11" t="s">
-        <v>833</v>
+      <c r="H328" s="16" t="s">
+        <v>827</v>
       </c>
       <c r="I328" s="12" t="s">
         <v>86</v>
@@ -15420,8 +15420,8 @@
       <c r="G399" s="11" t="s">
         <v>827</v>
       </c>
-      <c r="H399" s="11" t="s">
-        <v>79</v>
+      <c r="H399" s="16" t="s">
+        <v>827</v>
       </c>
       <c r="I399" s="12" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Améliration design pointage et compilation + Correction bug divers + Début modification systeme de sauvegarde.
</commit_message>
<xml_diff>
--- a/Symfony/Validation Manager WF RF MAJ NR 300516.xlsx
+++ b/Symfony/Validation Manager WF RF MAJ NR 300516.xlsx
@@ -3588,7 +3588,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3684,23 +3684,23 @@
   </sheetPr>
   <dimension ref="A1:N399"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A285" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H295" activeCellId="0" sqref="H295"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A317" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I328" activeCellId="0" sqref="I328"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.3214285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="24.7040816326531"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="256" min="10" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.9183673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="256" min="10" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="1" width="10.6632653061225"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -12379,11 +12379,11 @@
       <c r="G294" s="13" t="s">
         <v>827</v>
       </c>
-      <c r="H294" s="16" t="s">
+      <c r="H294" s="11" t="s">
         <v>827</v>
       </c>
-      <c r="I294" s="12" t="s">
-        <v>86</v>
+      <c r="I294" s="16" t="s">
+        <v>827</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13365,11 +13365,11 @@
       <c r="G328" s="13" t="s">
         <v>827</v>
       </c>
-      <c r="H328" s="16" t="s">
+      <c r="H328" s="11" t="s">
         <v>827</v>
       </c>
-      <c r="I328" s="12" t="s">
-        <v>86</v>
+      <c r="I328" s="16" t="s">
+        <v>827</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15420,11 +15420,11 @@
       <c r="G399" s="11" t="s">
         <v>827</v>
       </c>
-      <c r="H399" s="16" t="s">
+      <c r="H399" s="11" t="s">
         <v>827</v>
       </c>
-      <c r="I399" s="12" t="s">
-        <v>19</v>
+      <c r="I399" s="16" t="s">
+        <v>827</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fin modification formulaire demande materiel/logiciel.
</commit_message>
<xml_diff>
--- a/Symfony/Validation Manager WF RF MAJ NR 300516.xlsx
+++ b/Symfony/Validation Manager WF RF MAJ NR 300516.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3552" uniqueCount="1100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3543" uniqueCount="1100">
   <si>
     <t>Validation Manager WORKFLOW RH</t>
   </si>
@@ -2485,6 +2485,9 @@
     <t>TRISTAN</t>
   </si>
   <si>
+    <t>Nicolas RIGAUDEAU</t>
+  </si>
+  <si>
     <t>Laurent MORISSEAU</t>
   </si>
   <si>
@@ -2810,9 +2813,6 @@
   </si>
   <si>
     <t>FORESTIER</t>
-  </si>
-  <si>
-    <t>Nicolas RIGAUDEAU</t>
   </si>
   <si>
     <t>00000313</t>
@@ -3523,7 +3523,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3585,6 +3585,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3682,25 +3690,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:N399"/>
+  <dimension ref="A1:N65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A317" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I328" activeCellId="0" sqref="I328"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A313" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G328" activeCellId="0" sqref="G328"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.9183673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="256" min="10" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.515306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="256" min="10" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="1" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -12289,11 +12297,11 @@
       <c r="F291" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="G291" s="13" t="s">
-        <v>84</v>
+      <c r="G291" s="16" t="s">
+        <v>820</v>
       </c>
       <c r="H291" s="11" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="I291" s="12" t="s">
         <v>86</v>
@@ -12307,10 +12315,10 @@
         <v>786</v>
       </c>
       <c r="C292" s="11" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="D292" s="11" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="E292" s="11" t="s">
         <v>606</v>
@@ -12322,7 +12330,7 @@
         <v>84</v>
       </c>
       <c r="H292" s="11" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="I292" s="12" t="s">
         <v>86</v>
@@ -12336,13 +12344,13 @@
         <v>786</v>
       </c>
       <c r="C293" s="11" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="D293" s="11" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="E293" s="11" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="F293" s="11" t="s">
         <v>16</v>
@@ -12351,7 +12359,7 @@
         <v>84</v>
       </c>
       <c r="H293" s="11" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="I293" s="12" t="s">
         <v>86</v>
@@ -12365,7 +12373,7 @@
         <v>786</v>
       </c>
       <c r="C294" s="11" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="D294" s="11" t="s">
         <v>484</v>
@@ -12377,13 +12385,13 @@
         <v>16</v>
       </c>
       <c r="G294" s="13" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="H294" s="11" t="s">
-        <v>827</v>
-      </c>
-      <c r="I294" s="16" t="s">
-        <v>827</v>
+        <v>828</v>
+      </c>
+      <c r="I294" s="12" t="s">
+        <v>828</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12394,13 +12402,13 @@
         <v>786</v>
       </c>
       <c r="C295" s="11" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="D295" s="11" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="E295" s="11" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="F295" s="11" t="s">
         <v>34</v>
@@ -12409,7 +12417,7 @@
         <v>84</v>
       </c>
       <c r="H295" s="11" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="I295" s="12" t="s">
         <v>86</v>
@@ -12423,10 +12431,10 @@
         <v>786</v>
       </c>
       <c r="C296" s="11" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="D296" s="11" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="E296" s="11" t="s">
         <v>748</v>
@@ -12434,11 +12442,11 @@
       <c r="F296" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G296" s="13" t="s">
-        <v>84</v>
+      <c r="G296" s="16" t="s">
+        <v>820</v>
       </c>
       <c r="H296" s="11" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="I296" s="12" t="s">
         <v>86</v>
@@ -12452,13 +12460,13 @@
         <v>786</v>
       </c>
       <c r="C297" s="11" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="D297" s="11" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="E297" s="11" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="F297" s="11" t="s">
         <v>16</v>
@@ -12481,13 +12489,13 @@
         <v>786</v>
       </c>
       <c r="C298" s="11" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="D298" s="11" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="E298" s="11" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="F298" s="11" t="s">
         <v>16</v>
@@ -12510,13 +12518,13 @@
         <v>786</v>
       </c>
       <c r="C299" s="11" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="D299" s="11" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="E299" s="11" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="F299" s="11" t="s">
         <v>16</v>
@@ -12539,13 +12547,13 @@
         <v>786</v>
       </c>
       <c r="C300" s="11" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="D300" s="11" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="E300" s="11" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="F300" s="11" t="s">
         <v>16</v>
@@ -12568,13 +12576,13 @@
         <v>786</v>
       </c>
       <c r="C301" s="11" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="D301" s="11" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="E301" s="11" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="F301" s="11" t="s">
         <v>16</v>
@@ -12597,13 +12605,13 @@
         <v>786</v>
       </c>
       <c r="C302" s="11" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="D302" s="11" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="E302" s="11" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="F302" s="11" t="s">
         <v>16</v>
@@ -12626,10 +12634,10 @@
         <v>786</v>
       </c>
       <c r="C303" s="11" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="D303" s="11" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="E303" s="11" t="s">
         <v>78</v>
@@ -12652,22 +12660,22 @@
         <v>252</v>
       </c>
       <c r="B304" s="11" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="C304" s="11" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="D304" s="11" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="E304" s="11" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="F304" s="11" t="s">
         <v>16</v>
       </c>
       <c r="G304" s="11" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="H304" s="11" t="s">
         <v>18</v>
@@ -12681,25 +12689,25 @@
         <v>252</v>
       </c>
       <c r="B305" s="11" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="C305" s="11" t="s">
+        <v>860</v>
+      </c>
+      <c r="D305" s="11" t="s">
+        <v>861</v>
+      </c>
+      <c r="E305" s="11" t="s">
+        <v>862</v>
+      </c>
+      <c r="F305" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G305" s="11" t="s">
         <v>859</v>
       </c>
-      <c r="D305" s="11" t="s">
-        <v>860</v>
-      </c>
-      <c r="E305" s="11" t="s">
-        <v>861</v>
-      </c>
-      <c r="F305" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G305" s="11" t="s">
-        <v>858</v>
-      </c>
       <c r="H305" s="11" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="I305" s="12" t="s">
         <v>106</v>
@@ -12710,25 +12718,25 @@
         <v>252</v>
       </c>
       <c r="B306" s="11" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="C306" s="11" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="D306" s="11" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="E306" s="11" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="F306" s="11" t="s">
         <v>62</v>
       </c>
       <c r="G306" s="11" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="H306" s="11" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="I306" s="12" t="s">
         <v>106</v>
@@ -12739,25 +12747,25 @@
         <v>252</v>
       </c>
       <c r="B307" s="11" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="C307" s="11" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="D307" s="11" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="E307" s="11" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="F307" s="11" t="s">
         <v>16</v>
       </c>
       <c r="G307" s="11" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="H307" s="11" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="I307" s="12" t="s">
         <v>106</v>
@@ -12768,13 +12776,13 @@
         <v>252</v>
       </c>
       <c r="B308" s="11" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="C308" s="11" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="D308" s="11" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="E308" s="11" t="s">
         <v>299</v>
@@ -12783,10 +12791,10 @@
         <v>16</v>
       </c>
       <c r="G308" s="11" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="H308" s="11" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="I308" s="12" t="s">
         <v>106</v>
@@ -12797,25 +12805,25 @@
         <v>252</v>
       </c>
       <c r="B309" s="11" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="C309" s="11" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="D309" s="11" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="E309" s="11" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="F309" s="11" t="s">
         <v>16</v>
       </c>
       <c r="G309" s="11" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="H309" s="11" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="I309" s="12" t="s">
         <v>106</v>
@@ -12826,13 +12834,13 @@
         <v>252</v>
       </c>
       <c r="B310" s="11" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="C310" s="11" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="D310" s="11" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="E310" s="11" t="s">
         <v>420</v>
@@ -12841,10 +12849,10 @@
         <v>16</v>
       </c>
       <c r="G310" s="11" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="H310" s="11" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="I310" s="12" t="s">
         <v>106</v>
@@ -12855,25 +12863,25 @@
         <v>252</v>
       </c>
       <c r="B311" s="11" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="C311" s="11" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="D311" s="11" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="E311" s="11" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="F311" s="11" t="s">
         <v>16</v>
       </c>
       <c r="G311" s="11" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="H311" s="11" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="I311" s="12" t="s">
         <v>106</v>
@@ -12884,25 +12892,25 @@
         <v>252</v>
       </c>
       <c r="B312" s="11" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="C312" s="11" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="D312" s="11" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="E312" s="11" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="F312" s="11" t="s">
         <v>62</v>
       </c>
       <c r="G312" s="11" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="H312" s="11" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="I312" s="12" t="s">
         <v>106</v>
@@ -12913,13 +12921,13 @@
         <v>252</v>
       </c>
       <c r="B313" s="11" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="C313" s="11" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="D313" s="11" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="E313" s="11" t="s">
         <v>398</v>
@@ -12928,10 +12936,10 @@
         <v>16</v>
       </c>
       <c r="G313" s="11" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="H313" s="11" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="I313" s="12" t="s">
         <v>106</v>
@@ -12942,13 +12950,13 @@
         <v>252</v>
       </c>
       <c r="B314" s="11" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="C314" s="11" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="D314" s="11" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="E314" s="11" t="s">
         <v>447</v>
@@ -12957,10 +12965,10 @@
         <v>16</v>
       </c>
       <c r="G314" s="11" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="H314" s="11" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="I314" s="12" t="s">
         <v>106</v>
@@ -12968,19 +12976,19 @@
     </row>
     <row r="315" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A315" s="10" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B315" s="11" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C315" s="11" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="D315" s="11" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="E315" s="11" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="F315" s="11" t="s">
         <v>16</v>
@@ -12997,19 +13005,19 @@
     </row>
     <row r="316" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A316" s="10" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B316" s="11" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C316" s="11" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="D316" s="11" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="E316" s="11" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="F316" s="11" t="s">
         <v>16</v>
@@ -13026,16 +13034,16 @@
     </row>
     <row r="317" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A317" s="10" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B317" s="11" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C317" s="11" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="D317" s="11" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="E317" s="11" t="s">
         <v>555</v>
@@ -13055,16 +13063,16 @@
     </row>
     <row r="318" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A318" s="10" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B318" s="11" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C318" s="11" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="D318" s="11" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="E318" s="11" t="s">
         <v>305</v>
@@ -13084,19 +13092,19 @@
     </row>
     <row r="319" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A319" s="10" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B319" s="11" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C319" s="11" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="D319" s="11" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="E319" s="11" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="F319" s="11" t="s">
         <v>16</v>
@@ -13113,16 +13121,16 @@
     </row>
     <row r="320" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A320" s="10" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B320" s="11" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C320" s="11" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="D320" s="11" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="E320" s="11" t="s">
         <v>363</v>
@@ -13134,7 +13142,7 @@
         <v>84</v>
       </c>
       <c r="H320" s="11" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="I320" s="12" t="s">
         <v>86</v>
@@ -13142,19 +13150,19 @@
     </row>
     <row r="321" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A321" s="10" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B321" s="11" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C321" s="11" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="D321" s="11" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="E321" s="11" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="F321" s="11" t="s">
         <v>16</v>
@@ -13171,16 +13179,16 @@
     </row>
     <row r="322" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A322" s="10" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B322" s="11" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C322" s="11" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="D322" s="11" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="E322" s="11" t="s">
         <v>527</v>
@@ -13192,7 +13200,7 @@
         <v>84</v>
       </c>
       <c r="H322" s="11" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="I322" s="12" t="s">
         <v>86</v>
@@ -13200,16 +13208,16 @@
     </row>
     <row r="323" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A323" s="10" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B323" s="11" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C323" s="11" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="D323" s="11" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="E323" s="11" t="s">
         <v>595</v>
@@ -13221,7 +13229,7 @@
         <v>84</v>
       </c>
       <c r="H323" s="11" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="I323" s="12" t="s">
         <v>86</v>
@@ -13229,16 +13237,16 @@
     </row>
     <row r="324" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A324" s="10" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B324" s="11" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C324" s="11" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="D324" s="11" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="E324" s="11" t="s">
         <v>784</v>
@@ -13250,7 +13258,7 @@
         <v>84</v>
       </c>
       <c r="H324" s="11" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="I324" s="12" t="s">
         <v>86</v>
@@ -13258,16 +13266,16 @@
     </row>
     <row r="325" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A325" s="10" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B325" s="11" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C325" s="11" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="D325" s="11" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="E325" s="11" t="s">
         <v>162</v>
@@ -13279,7 +13287,7 @@
         <v>84</v>
       </c>
       <c r="H325" s="11" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="I325" s="12" t="s">
         <v>86</v>
@@ -13287,19 +13295,19 @@
     </row>
     <row r="326" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A326" s="10" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B326" s="11" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C326" s="11" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="D326" s="11" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="E326" s="11" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="F326" s="11" t="s">
         <v>34</v>
@@ -13316,19 +13324,19 @@
     </row>
     <row r="327" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A327" s="10" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B327" s="11" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C327" s="11" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="D327" s="11" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="E327" s="11" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="F327" s="11" t="s">
         <v>16</v>
@@ -13337,7 +13345,7 @@
         <v>84</v>
       </c>
       <c r="H327" s="11" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="I327" s="12" t="s">
         <v>86</v>
@@ -13345,16 +13353,16 @@
     </row>
     <row r="328" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A328" s="10" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B328" s="11" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C328" s="11" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="D328" s="11" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="E328" s="11" t="s">
         <v>78</v>
@@ -13362,28 +13370,28 @@
       <c r="F328" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G328" s="13" t="s">
-        <v>827</v>
-      </c>
-      <c r="H328" s="11" t="s">
-        <v>827</v>
-      </c>
-      <c r="I328" s="16" t="s">
-        <v>827</v>
+      <c r="G328" s="16" t="s">
+        <v>820</v>
+      </c>
+      <c r="H328" s="17" t="s">
+        <v>820</v>
+      </c>
+      <c r="I328" s="18" t="s">
+        <v>820</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A329" s="10" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B329" s="11" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C329" s="11" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="D329" s="11" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="E329" s="11" t="s">
         <v>299</v>
@@ -13395,7 +13403,7 @@
         <v>84</v>
       </c>
       <c r="H329" s="11" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="I329" s="12" t="s">
         <v>86</v>
@@ -13403,16 +13411,16 @@
     </row>
     <row r="330" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A330" s="10" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B330" s="11" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C330" s="11" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="D330" s="11" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="E330" s="11" t="s">
         <v>635</v>
@@ -13424,7 +13432,7 @@
         <v>84</v>
       </c>
       <c r="H330" s="11" t="s">
-        <v>929</v>
+        <v>820</v>
       </c>
       <c r="I330" s="12" t="s">
         <v>86</v>
@@ -13432,10 +13440,10 @@
     </row>
     <row r="331" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A331" s="10" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B331" s="11" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C331" s="11" t="s">
         <v>930</v>
@@ -13453,7 +13461,7 @@
         <v>84</v>
       </c>
       <c r="H331" s="11" t="s">
-        <v>929</v>
+        <v>820</v>
       </c>
       <c r="I331" s="12" t="s">
         <v>86</v>
@@ -13461,10 +13469,10 @@
     </row>
     <row r="332" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A332" s="10" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B332" s="11" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C332" s="11" t="s">
         <v>933</v>
@@ -13473,7 +13481,7 @@
         <v>934</v>
       </c>
       <c r="E332" s="11" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="F332" s="11" t="s">
         <v>34</v>
@@ -13482,7 +13490,7 @@
         <v>84</v>
       </c>
       <c r="H332" s="11" t="s">
-        <v>929</v>
+        <v>820</v>
       </c>
       <c r="I332" s="12" t="s">
         <v>86</v>
@@ -13490,10 +13498,10 @@
     </row>
     <row r="333" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A333" s="10" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B333" s="11" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C333" s="11" t="s">
         <v>935</v>
@@ -13511,7 +13519,7 @@
         <v>84</v>
       </c>
       <c r="H333" s="11" t="s">
-        <v>929</v>
+        <v>820</v>
       </c>
       <c r="I333" s="12" t="s">
         <v>86</v>
@@ -13519,10 +13527,10 @@
     </row>
     <row r="334" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A334" s="10" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B334" s="11" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C334" s="11" t="s">
         <v>938</v>
@@ -13548,10 +13556,10 @@
     </row>
     <row r="335" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A335" s="10" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B335" s="11" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C335" s="11" t="s">
         <v>942</v>
@@ -13577,10 +13585,10 @@
     </row>
     <row r="336" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A336" s="10" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B336" s="11" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C336" s="11" t="s">
         <v>946</v>
@@ -13606,10 +13614,10 @@
     </row>
     <row r="337" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A337" s="10" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B337" s="11" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C337" s="11" t="s">
         <v>949</v>
@@ -13635,10 +13643,10 @@
     </row>
     <row r="338" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A338" s="10" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B338" s="11" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C338" s="11" t="s">
         <v>952</v>
@@ -13664,10 +13672,10 @@
     </row>
     <row r="339" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A339" s="10" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B339" s="11" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C339" s="11" t="s">
         <v>955</v>
@@ -13693,10 +13701,10 @@
     </row>
     <row r="340" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A340" s="10" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B340" s="11" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C340" s="11" t="s">
         <v>957</v>
@@ -13722,10 +13730,10 @@
     </row>
     <row r="341" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A341" s="10" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B341" s="11" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C341" s="11" t="s">
         <v>960</v>
@@ -13751,10 +13759,10 @@
     </row>
     <row r="342" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A342" s="10" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B342" s="11" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C342" s="11" t="s">
         <v>963</v>
@@ -14050,7 +14058,7 @@
         <v>991</v>
       </c>
       <c r="D352" s="11" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="E352" s="11" t="s">
         <v>992</v>
@@ -14149,7 +14157,7 @@
         <v>993</v>
       </c>
       <c r="H355" s="11" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="I355" s="12" t="s">
         <v>19</v>
@@ -14178,7 +14186,7 @@
         <v>993</v>
       </c>
       <c r="H356" s="11" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="I356" s="12" t="s">
         <v>19</v>
@@ -14935,31 +14943,31 @@
       </c>
     </row>
     <row r="383" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A383" s="17" t="s">
+      <c r="A383" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="B383" s="18" t="s">
+      <c r="B383" s="20" t="s">
         <v>1052</v>
       </c>
-      <c r="C383" s="18" t="s">
+      <c r="C383" s="20" t="s">
         <v>1065</v>
       </c>
-      <c r="D383" s="18" t="s">
+      <c r="D383" s="20" t="s">
         <v>1066</v>
       </c>
-      <c r="E383" s="18" t="s">
+      <c r="E383" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="F383" s="18" t="s">
+      <c r="F383" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="G383" s="18" t="s">
+      <c r="G383" s="20" t="s">
         <v>68</v>
       </c>
       <c r="H383" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="I383" s="19" t="s">
+      <c r="I383" s="21" t="s">
         <v>19</v>
       </c>
     </row>
@@ -15180,7 +15188,7 @@
         <v>1084</v>
       </c>
       <c r="E391" s="11" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="F391" s="11" t="s">
         <v>16</v>
@@ -15398,35 +15406,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A399" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B399" s="10" t="s">
-        <v>1052</v>
-      </c>
-      <c r="C399" s="11" t="s">
-        <v>1097</v>
-      </c>
-      <c r="D399" s="11" t="s">
-        <v>542</v>
-      </c>
-      <c r="E399" s="11" t="s">
-        <v>819</v>
-      </c>
-      <c r="F399" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G399" s="11" t="s">
-        <v>827</v>
-      </c>
-      <c r="H399" s="11" t="s">
-        <v>827</v>
-      </c>
-      <c r="I399" s="16" t="s">
-        <v>827</v>
-      </c>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:I2"/>
@@ -15779,78 +15759,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A399:I399">
-    <cfRule type="colorScale" priority="31">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A399">
-    <cfRule type="colorScale" priority="32">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A399">
-    <cfRule type="colorScale" priority="33">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A399">
-    <cfRule type="colorScale" priority="34">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B399">
-    <cfRule type="colorScale" priority="35">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B399">
-    <cfRule type="colorScale" priority="36">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.784027777777778" right="0.784027777777778" top="0.980555555555556" bottom="0.980555555555556" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="9" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Avancement sur la recherche d'affaire par numéro et changement du système de suppression des colonnes d'affaires.
</commit_message>
<xml_diff>
--- a/Symfony/Validation Manager WF RF MAJ NR 300516.xlsx
+++ b/Symfony/Validation Manager WF RF MAJ NR 300516.xlsx
@@ -2485,46 +2485,46 @@
     <t>TRISTAN</t>
   </si>
   <si>
+    <t>Tristan BESSON</t>
+  </si>
+  <si>
+    <t>00000106</t>
+  </si>
+  <si>
+    <t>JUBEAU</t>
+  </si>
+  <si>
+    <t>Laurent MORISSEAU</t>
+  </si>
+  <si>
+    <t>00000411</t>
+  </si>
+  <si>
+    <t>LY</t>
+  </si>
+  <si>
+    <t>MARIE</t>
+  </si>
+  <si>
+    <t>00000089</t>
+  </si>
+  <si>
+    <t>00000466</t>
+  </si>
+  <si>
+    <t>THUREAU</t>
+  </si>
+  <si>
+    <t>CEDRIC</t>
+  </si>
+  <si>
+    <t>00000456</t>
+  </si>
+  <si>
+    <t>MORISSEAU</t>
+  </si>
+  <si>
     <t>Nicolas RIGAUDEAU</t>
-  </si>
-  <si>
-    <t>Laurent MORISSEAU</t>
-  </si>
-  <si>
-    <t>00000106</t>
-  </si>
-  <si>
-    <t>JUBEAU</t>
-  </si>
-  <si>
-    <t>00000411</t>
-  </si>
-  <si>
-    <t>LY</t>
-  </si>
-  <si>
-    <t>MARIE</t>
-  </si>
-  <si>
-    <t>00000089</t>
-  </si>
-  <si>
-    <t>Tristan BESSON</t>
-  </si>
-  <si>
-    <t>00000466</t>
-  </si>
-  <si>
-    <t>THUREAU</t>
-  </si>
-  <si>
-    <t>CEDRIC</t>
-  </si>
-  <si>
-    <t>00000456</t>
-  </si>
-  <si>
-    <t>MORISSEAU</t>
   </si>
   <si>
     <t>Lionel LEMARECHAL</t>
@@ -3523,7 +3523,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3589,14 +3589,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3692,23 +3684,23 @@
   </sheetPr>
   <dimension ref="A1:N65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A313" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G328" activeCellId="0" sqref="G328"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A283" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H291" activeCellId="0" sqref="H291"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.515306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="256" min="10" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="256" min="10" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="1" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -12297,11 +12289,11 @@
       <c r="F291" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="G291" s="16" t="s">
+      <c r="G291" s="13" t="s">
         <v>820</v>
       </c>
-      <c r="H291" s="11" t="s">
-        <v>821</v>
+      <c r="H291" s="16" t="s">
+        <v>820</v>
       </c>
       <c r="I291" s="12" t="s">
         <v>86</v>
@@ -12315,10 +12307,10 @@
         <v>786</v>
       </c>
       <c r="C292" s="11" t="s">
+        <v>821</v>
+      </c>
+      <c r="D292" s="11" t="s">
         <v>822</v>
-      </c>
-      <c r="D292" s="11" t="s">
-        <v>823</v>
       </c>
       <c r="E292" s="11" t="s">
         <v>606</v>
@@ -12330,7 +12322,7 @@
         <v>84</v>
       </c>
       <c r="H292" s="11" t="s">
-        <v>821</v>
+        <v>823</v>
       </c>
       <c r="I292" s="12" t="s">
         <v>86</v>
@@ -12359,7 +12351,7 @@
         <v>84</v>
       </c>
       <c r="H293" s="11" t="s">
-        <v>821</v>
+        <v>823</v>
       </c>
       <c r="I293" s="12" t="s">
         <v>86</v>
@@ -12385,13 +12377,13 @@
         <v>16</v>
       </c>
       <c r="G294" s="13" t="s">
-        <v>828</v>
+        <v>820</v>
       </c>
       <c r="H294" s="11" t="s">
-        <v>828</v>
+        <v>820</v>
       </c>
       <c r="I294" s="12" t="s">
-        <v>828</v>
+        <v>820</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12402,13 +12394,13 @@
         <v>786</v>
       </c>
       <c r="C295" s="11" t="s">
+        <v>828</v>
+      </c>
+      <c r="D295" s="11" t="s">
         <v>829</v>
       </c>
-      <c r="D295" s="11" t="s">
+      <c r="E295" s="11" t="s">
         <v>830</v>
-      </c>
-      <c r="E295" s="11" t="s">
-        <v>831</v>
       </c>
       <c r="F295" s="11" t="s">
         <v>34</v>
@@ -12417,7 +12409,7 @@
         <v>84</v>
       </c>
       <c r="H295" s="11" t="s">
-        <v>821</v>
+        <v>823</v>
       </c>
       <c r="I295" s="12" t="s">
         <v>86</v>
@@ -12431,10 +12423,10 @@
         <v>786</v>
       </c>
       <c r="C296" s="11" t="s">
+        <v>831</v>
+      </c>
+      <c r="D296" s="11" t="s">
         <v>832</v>
-      </c>
-      <c r="D296" s="11" t="s">
-        <v>833</v>
       </c>
       <c r="E296" s="11" t="s">
         <v>748</v>
@@ -12442,8 +12434,8 @@
       <c r="F296" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G296" s="16" t="s">
-        <v>820</v>
+      <c r="G296" s="13" t="s">
+        <v>833</v>
       </c>
       <c r="H296" s="11" t="s">
         <v>834</v>
@@ -13370,14 +13362,14 @@
       <c r="F328" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G328" s="16" t="s">
-        <v>820</v>
-      </c>
-      <c r="H328" s="17" t="s">
-        <v>820</v>
-      </c>
-      <c r="I328" s="18" t="s">
-        <v>820</v>
+      <c r="G328" s="13" t="s">
+        <v>833</v>
+      </c>
+      <c r="H328" s="11" t="s">
+        <v>833</v>
+      </c>
+      <c r="I328" s="12" t="s">
+        <v>833</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13432,7 +13424,7 @@
         <v>84</v>
       </c>
       <c r="H330" s="11" t="s">
-        <v>820</v>
+        <v>833</v>
       </c>
       <c r="I330" s="12" t="s">
         <v>86</v>
@@ -13461,7 +13453,7 @@
         <v>84</v>
       </c>
       <c r="H331" s="11" t="s">
-        <v>820</v>
+        <v>833</v>
       </c>
       <c r="I331" s="12" t="s">
         <v>86</v>
@@ -13490,7 +13482,7 @@
         <v>84</v>
       </c>
       <c r="H332" s="11" t="s">
-        <v>820</v>
+        <v>833</v>
       </c>
       <c r="I332" s="12" t="s">
         <v>86</v>
@@ -13519,7 +13511,7 @@
         <v>84</v>
       </c>
       <c r="H333" s="11" t="s">
-        <v>820</v>
+        <v>833</v>
       </c>
       <c r="I333" s="12" t="s">
         <v>86</v>
@@ -14943,31 +14935,31 @@
       </c>
     </row>
     <row r="383" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A383" s="19" t="s">
+      <c r="A383" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B383" s="20" t="s">
+      <c r="B383" s="18" t="s">
         <v>1052</v>
       </c>
-      <c r="C383" s="20" t="s">
+      <c r="C383" s="18" t="s">
         <v>1065</v>
       </c>
-      <c r="D383" s="20" t="s">
+      <c r="D383" s="18" t="s">
         <v>1066</v>
       </c>
-      <c r="E383" s="20" t="s">
+      <c r="E383" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="F383" s="20" t="s">
+      <c r="F383" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="G383" s="20" t="s">
+      <c r="G383" s="18" t="s">
         <v>68</v>
       </c>
       <c r="H383" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="I383" s="21" t="s">
+      <c r="I383" s="19" t="s">
         <v>19</v>
       </c>
     </row>
@@ -15188,7 +15180,7 @@
         <v>1084</v>
       </c>
       <c r="E391" s="11" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="F391" s="11" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Modification du système de récupération de la hiérarchie des tuilisateurs + Suppression du total des pourcentages par mois.
</commit_message>
<xml_diff>
--- a/Symfony/Validation Manager WF RF MAJ NR 300516.xlsx
+++ b/Symfony/Validation Manager WF RF MAJ NR 300516.xlsx
@@ -3523,7 +3523,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3589,6 +3589,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3684,23 +3692,23 @@
   </sheetPr>
   <dimension ref="A1:N65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A283" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H291" activeCellId="0" sqref="H291"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A317" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F321" activeCellId="0" sqref="F321"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="256" min="10" style="1" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="256" min="10" style="1" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="1" width="10.2602040816327"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -12292,7 +12300,7 @@
       <c r="G291" s="13" t="s">
         <v>820</v>
       </c>
-      <c r="H291" s="16" t="s">
+      <c r="H291" s="11" t="s">
         <v>820</v>
       </c>
       <c r="I291" s="12" t="s">
@@ -13362,14 +13370,14 @@
       <c r="F328" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G328" s="13" t="s">
-        <v>833</v>
-      </c>
-      <c r="H328" s="11" t="s">
-        <v>833</v>
-      </c>
-      <c r="I328" s="12" t="s">
-        <v>833</v>
+      <c r="G328" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="H328" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="I328" s="18" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14935,31 +14943,31 @@
       </c>
     </row>
     <row r="383" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A383" s="17" t="s">
+      <c r="A383" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="B383" s="18" t="s">
+      <c r="B383" s="20" t="s">
         <v>1052</v>
       </c>
-      <c r="C383" s="18" t="s">
+      <c r="C383" s="20" t="s">
         <v>1065</v>
       </c>
-      <c r="D383" s="18" t="s">
+      <c r="D383" s="20" t="s">
         <v>1066</v>
       </c>
-      <c r="E383" s="18" t="s">
+      <c r="E383" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="F383" s="18" t="s">
+      <c r="F383" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="G383" s="18" t="s">
+      <c r="G383" s="20" t="s">
         <v>68</v>
       </c>
       <c r="H383" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="I383" s="19" t="s">
+      <c r="I383" s="21" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ajout de la gestion des jours fériés sur les pointages + Ajout de liens vers la gestion des pointages dans l'administration.
</commit_message>
<xml_diff>
--- a/Symfony/Validation Manager WF RF MAJ NR 300516.xlsx
+++ b/Symfony/Validation Manager WF RF MAJ NR 300516.xlsx
@@ -3523,7 +3523,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3585,14 +3585,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3692,23 +3684,23 @@
   </sheetPr>
   <dimension ref="A1:N65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A317" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F321" activeCellId="0" sqref="F321"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A277" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I291" activeCellId="0" sqref="I291"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="256" min="10" style="1" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="256" min="10" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="1" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -12303,8 +12295,8 @@
       <c r="H291" s="11" t="s">
         <v>820</v>
       </c>
-      <c r="I291" s="12" t="s">
-        <v>86</v>
+      <c r="I291" s="16" t="s">
+        <v>820</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13370,13 +13362,13 @@
       <c r="F328" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G328" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="H328" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="I328" s="18" t="s">
+      <c r="G328" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="H328" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="I328" s="12" t="s">
         <v>106</v>
       </c>
     </row>
@@ -14943,31 +14935,31 @@
       </c>
     </row>
     <row r="383" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A383" s="19" t="s">
+      <c r="A383" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B383" s="20" t="s">
+      <c r="B383" s="18" t="s">
         <v>1052</v>
       </c>
-      <c r="C383" s="20" t="s">
+      <c r="C383" s="18" t="s">
         <v>1065</v>
       </c>
-      <c r="D383" s="20" t="s">
+      <c r="D383" s="18" t="s">
         <v>1066</v>
       </c>
-      <c r="E383" s="20" t="s">
+      <c r="E383" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="F383" s="20" t="s">
+      <c r="F383" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="G383" s="20" t="s">
+      <c r="G383" s="18" t="s">
         <v>68</v>
       </c>
       <c r="H383" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="I383" s="21" t="s">
+      <c r="I383" s="19" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fin de l'ajout des headers flotants.
</commit_message>
<xml_diff>
--- a/Symfony/Validation Manager WF RF MAJ NR 300516.xlsx
+++ b/Symfony/Validation Manager WF RF MAJ NR 300516.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="226">
   <si>
     <t>Validation Manager WORKFLOW RH</t>
   </si>
@@ -698,6 +698,9 @@
   </si>
   <si>
     <t>TRISTAN</t>
+  </si>
+  <si>
+    <t>Tristan BESSON</t>
   </si>
 </sst>
 </file>
@@ -708,7 +711,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -763,11 +766,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -891,7 +889,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -950,10 +948,6 @@
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1036,23 +1030,23 @@
   </sheetPr>
   <dimension ref="A1:I135"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A124" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E143" activeCellId="0" sqref="E143"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A119" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D139" activeCellId="0" sqref="D139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.7295918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="256" min="10" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="1" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.3214285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="256" min="10" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="1" width="10.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -4888,8 +4882,8 @@
       <c r="F135" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G135" s="15" t="s">
-        <v>55</v>
+      <c r="G135" s="11" t="s">
+        <v>225</v>
       </c>
       <c r="H135" s="11" t="s">
         <v>220</v>

</xml_diff>